<commit_message>
power data additions made
</commit_message>
<xml_diff>
--- a/PowerData/fig8_67straight_67curve_10.8laps.xlsx
+++ b/PowerData/fig8_67straight_67curve_10.8laps.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bryantlj\Desktop\PanamaCityBeach\PowerData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1C4A1C6-3D5B-4EC6-A175-8BFBCC6DD2AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7E77147-084A-42CF-A6D1-2CD49EB15733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -8067,7 +8067,7 @@
   <dimension ref="A1:J239"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="74" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="S5" sqref="S5"/>
+      <selection activeCell="F1" activeCellId="1" sqref="A1:A1048576 F1:F1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>